<commit_message>
adding and updating RV64VCSR,RV64ZICSR,RV64PMA and RV64ZICBOM
</commit_message>
<xml_diff>
--- a/testplans/RV64Zicbom.xlsx
+++ b/testplans/RV64Zicbom.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="113">
   <si>
     <t>Sr No
 (link to coverage)</t>
@@ -37,7 +37,7 @@
     <t>Coverage Method</t>
   </si>
   <si>
-    <t>cover points written</t>
+    <t>Cover points written</t>
   </si>
   <si>
     <t>Feature covered</t>
@@ -90,15 +90,15 @@
     <t xml:space="preserve">
 Set up two virtual address VA1 and VA2 that should corespond to a same physical address PA each with different memory attributes. VA1 with cacheability, set and VA2 with non cacheable memory access set using PBMT bits. 
     • Do a store on VA1 with the value X and repeat it for whole cache line 
-    • Excute the CBO.INVAL using VA1
+    • Execute the CBO.INVAL using VA1
     • Do a load from VA2
 </t>
   </si>
   <si>
-    <t xml:space="preserve">check if the initial value is returned from the load operation because invalide operation </t>
+    <t xml:space="preserve">check if the initial value is returned from the load operation because of invalide operation </t>
   </si>
   <si>
-    <t>Testcase</t>
+    <t>Sellf Checking Test</t>
   </si>
   <si>
     <t>N/A</t>
@@ -479,6 +479,9 @@
  - For leaf PTE at level1 set pte.ppn[0] != 0 and test for write access. (For sv32, 39, 48 &amp; 57) on cache block
 Note:
  - Set pte.U=0 when test in Supervisor mode and Set pte.U=1 when testing in user mode."</t>
+  </si>
+  <si>
+    <t>cover points written</t>
   </si>
   <si>
     <t>pmp.1</t>
@@ -997,15 +1000,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.13"/>
-    <col customWidth="1" min="2" max="2" width="18.75"/>
-    <col customWidth="1" min="3" max="3" width="32.88"/>
+    <col customWidth="1" min="1" max="1" width="14.75"/>
+    <col customWidth="1" min="2" max="2" width="12.88"/>
+    <col customWidth="1" min="3" max="3" width="32.38"/>
     <col customWidth="1" min="4" max="4" width="80.75"/>
-    <col customWidth="1" min="5" max="5" width="51.0"/>
-    <col customWidth="1" min="6" max="6" width="21.75"/>
+    <col customWidth="1" min="5" max="5" width="49.25"/>
+    <col customWidth="1" min="6" max="6" width="17.75"/>
     <col customWidth="1" min="7" max="7" width="17.25"/>
-    <col customWidth="1" min="8" max="9" width="12.88"/>
-    <col customWidth="1" min="10" max="10" width="23.75"/>
+    <col customWidth="1" min="8" max="8" width="12.88"/>
+    <col customWidth="1" min="9" max="9" width="7.38"/>
+    <col customWidth="1" min="10" max="10" width="9.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -28522,14 +28526,14 @@
     <mergeCell ref="B19:B29"/>
   </mergeCells>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G29">
+      <formula1>"Sellf Checking Test,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F29">
       <formula1>"Self Checking,Signature Check,Check against RM,Coverage checks,Assertion Check,Any/All,N/A"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H22 H23:I29">
       <formula1>"Done,To be Done,N/A"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G29">
-      <formula1>"Testcase,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I22">
       <formula1>"Covered,Not covered"</formula1>
@@ -28581,7 +28585,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -28592,19 +28596,19 @@
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>15</v>
@@ -28620,17 +28624,17 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
updating the RV64CSR, RV64PMA, RV64zicbom
</commit_message>
<xml_diff>
--- a/testplans/RV64Zicbom.xlsx
+++ b/testplans/RV64Zicbom.xlsx
@@ -3,8 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="zicbom" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="zicbom_PMP" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Zicbom" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Zicbom_VM" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Zicbom_Svpbmt" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Zicbom_PMP" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="124">
   <si>
     <t>Sr No
 (link to coverage)</t>
@@ -55,11 +57,12 @@
     <t>illegal instruction exception</t>
   </si>
   <si>
-    <t>Execute the CBO.INVAL instruction when current privelege mode != M and menvcfg.CBIE = 00</t>
+    <t>Execute the CBO.INVAL instruction when menvcfg.CBIE = 00 for:
+-current privilege mode = S mode
+-current privilege mode = U mode</t>
   </si>
   <si>
-    <t>check if illegal instruction exception raised
-mcause.exception == 2</t>
+    <t>illegal instruction exception is raised</t>
   </si>
   <si>
     <t>Check against RM</t>
@@ -74,11 +77,10 @@
     <t>inv.2</t>
   </si>
   <si>
-    <t>Execute the CBO.INVAL instruction when current privelege mode = U and senvcfg.CBIE = 00</t>
+    <t>Execute the CBO.INVAL instruction when current privilege mode = U and senvcfg.CBIE = 00</t>
   </si>
   <si>
-    <t>check if illegal instruction exception raised
-Mcause.exception == 2</t>
+    <t xml:space="preserve"> illegal instruction exception raised</t>
   </si>
   <si>
     <t>inv.3</t>
@@ -88,14 +90,13 @@
   </si>
   <si>
     <t xml:space="preserve">
-Set up two virtual address VA1 and VA2 that should corespond to a same physical address PA each with different memory attributes. VA1 with cacheability, set and VA2 with non cacheable memory access set using PBMT bits. 
-    • Do a store on VA1 with the value X and repeat it for whole cache line 
-    • Execute the CBO.INVAL using VA1
-    • Do a load from VA2
+-Write to a cachable memory location
+ -Execute the CBO.INVAL 
+    -Do a load for the same memory location directly from main memory
 </t>
   </si>
   <si>
-    <t xml:space="preserve">check if the initial value is returned from the load operation because of invalide operation </t>
+    <t xml:space="preserve">Initial value is returned from the load operation </t>
   </si>
   <si>
     <t>Sellf Checking Test</t>
@@ -111,18 +112,20 @@
   </si>
   <si>
     <t xml:space="preserve">
-Execute the CBO.INVAL instruction when current privelege mode != M mode and menvcf.CBIE =01
+Execute the CBO.INVAL instruction when menvcf.CBIE =01 for:
+-current privilege mode = S mode
+-current privilege mode = U mode
 </t>
   </si>
   <si>
-    <t>check if the  CBO.FLUSH operation is performed</t>
+    <t>check if CBO.FLUSH operation is performed</t>
   </si>
   <si>
     <t>inv.5</t>
   </si>
   <si>
     <t xml:space="preserve">
-Execute the CBO.INVAL instruction when current privelege mode = U mode and senvcf.CBIE =01
+Execute the CBO.INVAL instruction when current privilege mode = U mode and senvcf.CBIE =01
 </t>
   </si>
   <si>
@@ -130,17 +133,18 @@
   </si>
   <si>
     <t xml:space="preserve">
-Execute the CBO.INVAL instruction when current privelege mode != M mode and menvcf.CBIE =11
-</t>
+Execute the CBO.INVAL instruction when menvcf.CBIE =11 for:
+-current privilege mode = S mode
+-current privilege mode = U mode</t>
   </si>
   <si>
-    <t>check if the  CBO.INVAL operation is performed</t>
+    <t>check if CBO.INVAL operation is performed</t>
   </si>
   <si>
     <t>inv.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Execute the CBO.INVAL instruction when current privelege mode = U mode and senvcf.CBIE =11
+    <t xml:space="preserve">Execute the CBO.INVAL instruction when current privilege mode = U mode and senvcf.CBIE =11
 </t>
   </si>
   <si>
@@ -153,13 +157,18 @@
     <t xml:space="preserve"> illegal instruction exception</t>
   </si>
   <si>
-    <t>Execute the CBO.CLEAN instruction when current privelege mode != M and !menvcfg.CBCFE</t>
+    <t>Execute the CBO.CLEAN instruction when !menvcfg.CBCFE for:
+-current privilege mode = S mode
+-current privilege mode = U mode</t>
+  </si>
+  <si>
+    <t>illegal instruction exception raised</t>
   </si>
   <si>
     <t>cl.2</t>
   </si>
   <si>
-    <t>Execute the CBO.CLEAN instruction when current privelege mode = U and !senvcfg.CBCFE</t>
+    <t>Execute the CBO.CLEAN instruction when current privilege mode = U and !senvcfg.CBCFE</t>
   </si>
   <si>
     <t>cl.3</t>
@@ -168,14 +177,12 @@
     <t>Clean operation</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Set up two virtual address VA1 and VA2 coresponding to same physical address PA each with different memory attributes. VA1 with cacheability and VA2 with non cacheable memory access set using PBMT bits. 
-    • Do a store on address A using VA1 and repeat it for whole cache line with the value X
-    • Excute the CBO.CLEAN using VA1
-    • Do a load from VA2. It will directly access memory</t>
+    <t>-Write to a cachable memory location with value X
+ -Execute the CBO.CLEAN
+    -Do a load for the same memory location directly from main memory</t>
   </si>
   <si>
-    <t>check if the same value X is returned from the load operation</t>
+    <t>Value X must be returned from the load operation</t>
   </si>
   <si>
     <t>cl.4</t>
@@ -185,18 +192,20 @@
   </si>
   <si>
     <t xml:space="preserve">
-Execute the CBO.CLEAN instruction when priv_mode != M mode and menvcf.CBCFE
+Execute the CBO.CLEAN instruction when menvcf.CBCFE for:
+-current privilege mode = S mode
+-current privilege mode = U mode
 </t>
   </si>
   <si>
-    <t>check if the  CBO.CLEAN operation is performed</t>
+    <t>check if CBO.CLEAN operation is performed</t>
   </si>
   <si>
     <t>cl.5</t>
   </si>
   <si>
     <t xml:space="preserve">
-Execute the CBO.CLEAN instruction when current privelege mode = U mode and senvcf.CBCFE
+Execute the CBO.CLEAN instruction when current privilege mode = U mode and senvcf.CBCFE
 </t>
   </si>
   <si>
@@ -206,13 +215,15 @@
     <t>CBO.FLUSH</t>
   </si>
   <si>
-    <t>Execute the CBO.FLUSH instruction when current privelege mode != M and !menvcfg.CBCFE</t>
+    <t>Execute the CBO.FLUSH instruction when !menvcfg.CBCFE for:
+-current privilege mode = S mode
+-current privilege mode = U mode</t>
   </si>
   <si>
     <t>fl.2</t>
   </si>
   <si>
-    <t>Execute the CBO.FLUSH instruction when current privelege mode = U and !senvcfg.CBCFE</t>
+    <t>Execute the CBO.FLUSH instruction when current privilege mode = U and !senvcfg.CBCFE</t>
   </si>
   <si>
     <t>fl.3</t>
@@ -221,19 +232,9 @@
     <t>Flush operation</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Set up two virtual address VA1 and VA2 coresponding to same physical address PA, each with different memory attributes. VA1 with cacheability and VA2 with non cacheable memory access set using PBMT bits. 
-    • Do a store on VA1 with the value X and repeat it for whole cache line 
-    • Excute the CBO.FLUSH using VA1
-    • Do a load1 from VA2
-    • Do store on VA2 with value Y
-    • Do a load2 from VA1
-</t>
-  </si>
-  <si>
-    <t>check if 
-    • The same value X is returned from the load1 operation and 
-    • Same value Y is returned from load2</t>
+    <t>-Write to a cachable memory location with value X
+ -Execute the CBO.FLUSH
+    -Do a load for the same memory location directly from main memory</t>
   </si>
   <si>
     <t>fl.4</t>
@@ -242,14 +243,19 @@
     <t>Behaviour of CBO.FLUSH with CSR</t>
   </si>
   <si>
-    <t xml:space="preserve">Execute the CBO.FLUSH instruction when priv_mode != M mode and menvcf.CBCFE
+    <t xml:space="preserve">Execute the CBO.FLUSH instruction when menvcf.CBCFE for:
+-current privilege mode = S mode
+-current privilege mode = U mode
 </t>
+  </si>
+  <si>
+    <t>check if the CBO.FLUSH operation is performed</t>
   </si>
   <si>
     <t>fl.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Execute the CBO.FLUSH instruction when priv_mode = U mode and senvcf.CBCFE
+    <t xml:space="preserve">Execute the CBO.FLUSH instruction when current privilege mode = U mode and senvcf.CBCFE
 </t>
   </si>
   <si>
@@ -431,7 +437,7 @@
  - All PMP permissions on targated pages if PMP is enabled
  - Valid leaf PTE, with no invalid RWX encoding
  - Execute sfence.vma before accessign the PTE.
-Test Cases:
+Test Cases: 
  - Set PTE.R=1 and PTE.W=1 &amp; pte.a=0 and test the write access on cache block
 Note:
  - For testing at level0, set all the pte perimssions at higher levels to 0 except PTE.v, so that non-leaf level points to level0.
@@ -479,6 +485,54 @@
  - For leaf PTE at level1 set pte.ppn[0] != 0 and test for write access. (For sv32, 39, 48 &amp; 57) on cache block
 Note:
  - Set pte.U=0 when test in Supervisor mode and Set pte.U=1 when testing in user mode."</t>
+  </si>
+  <si>
+    <t>pbmt.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Set up two virtual address VA1 and VA2 that should corespond to a same physical address PA each with different memory attributes. VA1 with cacheability, set and VA2 with non cacheable memory access set using PBMT bits. 
+    • Do a store on VA1 with the value X and repeat it for whole cache line 
+    • Execute the CBO.INVAL using VA1
+    • Do a load from VA2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check if the initial value is returned from the load operation because of invalide operation </t>
+  </si>
+  <si>
+    <t>Self Checking Test</t>
+  </si>
+  <si>
+    <t>pbmt.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Set up two virtual address VA1 and VA2 coresponding to same physical address PA each with different memory attributes. VA1 with cacheability and VA2 with non cacheable memory access set using PBMT bits. 
+    • Do a store on address A using VA1 and repeat it for whole cache line with the value X
+    • Excute the CBO.CLEAN using VA1
+    • Do a load from VA2. It will directly access memory</t>
+  </si>
+  <si>
+    <t>check if the same value X is returned from the load operation</t>
+  </si>
+  <si>
+    <t>pbmt.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Set up two virtual address VA1 and VA2 coresponding to same physical address PA, each with different memory attributes. VA1 with cacheability and VA2 with non cacheable memory access set using PBMT bits. 
+    • Do a store on VA1 with the value X and repeat it for whole cache line 
+    • Excute the CBO.FLUSH using VA1
+    • Do a load1 from VA2
+    • Do store on VA2 with value Y
+    • Do a load2 from VA1
+</t>
+  </si>
+  <si>
+    <t>check if 
+    • The same value X is returned from the load1 operation and 
+    • Same value Y is returned from load2</t>
   </si>
   <si>
     <t>cover points written</t>
@@ -598,18 +652,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -643,9 +697,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -654,22 +705,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -678,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -709,55 +744,43 @@
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
@@ -765,10 +788,7 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -790,6 +810,14 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1003,7 +1031,7 @@
     <col customWidth="1" min="1" max="1" width="14.75"/>
     <col customWidth="1" min="2" max="2" width="12.88"/>
     <col customWidth="1" min="3" max="3" width="32.38"/>
-    <col customWidth="1" min="4" max="4" width="80.75"/>
+    <col customWidth="1" min="4" max="4" width="76.75"/>
     <col customWidth="1" min="5" max="5" width="49.25"/>
     <col customWidth="1" min="6" max="6" width="17.75"/>
     <col customWidth="1" min="7" max="7" width="17.25"/>
@@ -1154,10 +1182,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1173,7 +1201,7 @@
         <v>26</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1197,13 +1225,13 @@
         <v>27</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -1216,7 +1244,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="15"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1240,13 +1268,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -1259,7 +1287,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="15"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -1283,13 +1311,13 @@
         <v>33</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -1302,7 +1330,7 @@
         <v>17</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="15"/>
+      <c r="J7" s="16"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -1325,14 +1353,14 @@
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1345,7 +1373,7 @@
         <v>17</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="15"/>
+      <c r="J8" s="16"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -1378,7 +1406,7 @@
         <v>41</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>15</v>
@@ -1411,17 +1439,17 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>15</v>
@@ -1454,17 +1482,17 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>47</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>15</v>
@@ -1476,7 +1504,7 @@
         <v>26</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1497,17 +1525,17 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>51</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>15</v>
@@ -1519,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="10"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="16"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1540,17 +1568,17 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>51</v>
+      <c r="B13" s="17"/>
+      <c r="C13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>15</v>
@@ -1562,7 +1590,7 @@
         <v>17</v>
       </c>
       <c r="I13" s="10"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1583,19 +1611,19 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>15</v>
@@ -1628,17 +1656,17 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>15</v>
@@ -1671,17 +1699,17 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="13" t="s">
         <v>61</v>
       </c>
+      <c r="D16" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>15</v>
@@ -1693,7 +1721,7 @@
         <v>26</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1717,14 +1745,14 @@
         <v>63</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>30</v>
+      <c r="E17" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>15</v>
@@ -1736,7 +1764,7 @@
         <v>17</v>
       </c>
       <c r="I17" s="10"/>
-      <c r="J17" s="15"/>
+      <c r="J17" s="16"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1757,17 +1785,17 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>67</v>
+      <c r="D18" s="15" t="s">
+        <v>68</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>30</v>
+      <c r="E18" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>15</v>
@@ -1779,7 +1807,7 @@
         <v>17</v>
       </c>
       <c r="I18" s="10"/>
-      <c r="J18" s="15"/>
+      <c r="J18" s="16"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -1799,32 +1827,6 @@
       <c r="AA18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="21"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -1844,30 +1846,6 @@
       <c r="AA19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="21"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -1887,30 +1865,6 @@
       <c r="AA20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="21"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
@@ -1930,30 +1884,6 @@
       <c r="AA21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="21"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -1973,30 +1903,6 @@
       <c r="AA22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="21"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -2016,30 +1922,6 @@
       <c r="AA23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="21"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -2059,30 +1941,6 @@
       <c r="AA24" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="21"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -2102,30 +1960,6 @@
       <c r="AA25" s="5"/>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="21"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -2145,30 +1979,6 @@
       <c r="AA26" s="5"/>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="21"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -2188,30 +1998,6 @@
       <c r="AA27" s="5"/>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="21"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -2231,30 +2017,6 @@
       <c r="AA28" s="5"/>
     </row>
     <row r="29">
-      <c r="A29" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="21"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
@@ -2334,8 +2096,8 @@
     <row r="32">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2655,7 +2417,7 @@
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="27"/>
+      <c r="E43" s="19"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -2684,7 +2446,7 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="27"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
@@ -28519,23 +28281,22 @@
       <c r="AA934" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B29"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G29">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G18">
       <formula1>"Sellf Checking Test,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F29">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F18">
       <formula1>"Self Checking,Signature Check,Check against RM,Coverage checks,Assertion Check,Any/All,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H22 H23:I29">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H18">
       <formula1>"Done,To be Done,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I22">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I18">
       <formula1>"Covered,Not covered"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28544,6 +28305,611 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="14.75"/>
+    <col customWidth="1" min="2" max="2" width="11.63"/>
+    <col customWidth="1" min="3" max="3" width="27.75"/>
+    <col customWidth="1" min="4" max="4" width="82.5"/>
+    <col customWidth="1" min="5" max="5" width="40.0"/>
+    <col customWidth="1" min="6" max="6" width="16.75"/>
+    <col customWidth="1" min="7" max="7" width="16.25"/>
+    <col customWidth="1" min="8" max="8" width="11.13"/>
+    <col customWidth="1" min="9" max="9" width="7.38"/>
+    <col customWidth="1" min="10" max="10" width="9.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B12"/>
+  </mergeCells>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G12">
+      <formula1>"Sellf Checking Test,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F12">
+      <formula1>"Self Checking,Signature Check,Check against RM,Coverage checks,Assertion Check,Any/All,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H5 H6:I12">
+      <formula1>"Done,To be Done,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I5">
+      <formula1>"Covered,Not covered"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="8.88"/>
+    <col customWidth="1" min="2" max="3" width="10.63"/>
+    <col customWidth="1" min="4" max="4" width="84.5"/>
+    <col customWidth="1" min="5" max="5" width="31.63"/>
+    <col customWidth="1" min="6" max="6" width="16.75"/>
+    <col customWidth="1" min="7" max="7" width="19.88"/>
+    <col customWidth="1" min="8" max="8" width="11.13"/>
+    <col customWidth="1" min="9" max="9" width="7.38"/>
+    <col customWidth="1" min="10" max="10" width="9.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F4">
+      <formula1>"Self Checking,Signature Check,Check against RM,Coverage checks,Assertion Check,Any/All,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H4">
+      <formula1>"Done,To be Done,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G4">
+      <formula1>"Self Checking Test,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I4">
+      <formula1>"Covered,Not covered"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -28585,7 +28951,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -28595,20 +28961,20 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="28" t="s">
-        <v>105</v>
+      <c r="A2" s="24" t="s">
+        <v>116</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>106</v>
+      <c r="B2" s="25" t="s">
+        <v>117</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>107</v>
+      <c r="C2" s="22" t="s">
+        <v>118</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>108</v>
+      <c r="D2" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>15</v>
@@ -28619,22 +28985,22 @@
       <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3">
-      <c r="A3" s="28" t="s">
-        <v>110</v>
+      <c r="A3" s="24" t="s">
+        <v>121</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="30" t="s">
-        <v>111</v>
+      <c r="B3" s="17"/>
+      <c r="C3" s="22" t="s">
+        <v>122</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>112</v>
+      <c r="D3" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>15</v>
@@ -28645,8 +29011,8 @@
       <c r="H3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>